<commit_message>
Created seperate files for better readability
</commit_message>
<xml_diff>
--- a/data/dataset_complete.xlsx
+++ b/data/dataset_complete.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\om\code\Valorant-Agent-Picker\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Om\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC8C1A23-E670-4B6B-B44B-721EAB98A29A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21CE7104-FDCD-4B59-977D-3C1F1C80FE7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2685" yWindow="2685" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -537,8 +537,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A967" workbookViewId="0">
-      <selection activeCell="U992" sqref="U992"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>